<commit_message>
Updated "WestSteep" model metrics
</commit_message>
<xml_diff>
--- a/inst/extdata/MetricNames.xlsx
+++ b/inst/extdata/MetricNames.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{DA5D9DE8-8857-49A5-893A-8DE2F5EA67A0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{D9BFB810-A492-40A7-9774-6C3C96A7E644}"/>
   <bookViews>
-    <workbookView xWindow="-19280" yWindow="-80" windowWidth="19360" windowHeight="10360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MetricMetadata" sheetId="3" r:id="rId1"/>
@@ -2758,7 +2758,7 @@
   <dimension ref="A1:G295"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B84" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="B237" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="B84" sqref="B84"/>

</xml_diff>

<commit_message>
Updated WestSteep Index Region
Updated metrics for WestSteep Index Region. pi_EPT is a placeholder for pi_EPTnoBH until it's defined by Jessup. All metrics are correct but selection in metric.values.R is not correct.
</commit_message>
<xml_diff>
--- a/inst/extdata/MetricNames.xlsx
+++ b/inst/extdata/MetricNames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben.Block\OneDrive - Tetra Tech, Inc\GitHub\BioMonTools\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{DA5D9DE8-8857-49A5-893A-8DE2F5EA67A0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{A1425F31-DCAE-4B5F-998E-D8EEC0A37EB2}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{DA5D9DE8-8857-49A5-893A-8DE2F5EA67A0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{5288D484-74D7-41B4-850B-A00069A3F7ED}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="NOTES" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MetricMetadata!$A$5:$G$295</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MetricMetadata!$A$5:$G$296</definedName>
     <definedName name="FileName" localSheetId="1">NOTES!$B$8</definedName>
     <definedName name="FileName">#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">MetricMetadata!$A:$A,MetricMetadata!$5:$5</definedName>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1194" uniqueCount="660">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1199" uniqueCount="662">
   <si>
     <t>nt_total</t>
   </si>
@@ -2083,6 +2083,12 @@
   </si>
   <si>
     <t>Added one metric for MI EGLE: pi_IsoMolHir [input by Ben Block, Tt]</t>
+  </si>
+  <si>
+    <t>pi_EPTnoBH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">percent (0-100) individuals - Orders Ephemeroptera, Plecoptera and Trichoptera (EPT) and not </t>
   </si>
 </sst>
 </file>
@@ -2204,7 +2210,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2232,6 +2238,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2289,7 +2301,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2389,6 +2401,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2755,13 +2782,13 @@
   <sheetPr codeName="Sheet3">
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:G295"/>
+  <dimension ref="A1:G296"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B65" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="B36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B75" sqref="B75"/>
+      <selection pane="bottomRight" activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2801,8 +2828,8 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="24">
-        <f>SUBTOTAL(3,A6:A295)</f>
-        <v>290</v>
+        <f>SUBTOTAL(3,A6:A296)</f>
+        <v>291</v>
       </c>
       <c r="G3" s="38" t="s">
         <v>541</v>
@@ -3679,37 +3706,39 @@
       <c r="D55" s="16"/>
       <c r="E55" s="16"/>
       <c r="F55" s="9"/>
-      <c r="G55" s="1"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="7" t="s">
+      <c r="G55" s="1" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="39" t="s">
+        <v>660</v>
+      </c>
+      <c r="B56" s="39" t="s">
+        <v>661</v>
+      </c>
+      <c r="C56" s="16" t="s">
+        <v>641</v>
+      </c>
+      <c r="D56" s="40"/>
+      <c r="E56" s="40"/>
+      <c r="F56" s="41"/>
+      <c r="G56" s="42" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="B57" s="7" t="s">
         <v>382</v>
       </c>
-      <c r="C56" s="16" t="s">
+      <c r="C57" s="16" t="s">
         <v>240</v>
       </c>
-      <c r="D56" s="16"/>
-      <c r="E56" s="16"/>
-      <c r="F56" s="9"/>
-      <c r="G56" s="1" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="10" t="s">
-        <v>326</v>
-      </c>
-      <c r="B57" s="10" t="s">
-        <v>383</v>
-      </c>
-      <c r="C57" s="16" t="s">
-        <v>641</v>
-      </c>
-      <c r="D57" s="20"/>
-      <c r="E57" s="20"/>
+      <c r="D57" s="16"/>
+      <c r="E57" s="16"/>
       <c r="F57" s="9"/>
       <c r="G57" s="1" t="s">
         <v>539</v>
@@ -3717,10 +3746,10 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
-        <v>514</v>
+        <v>326</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>516</v>
+        <v>383</v>
       </c>
       <c r="C58" s="16" t="s">
         <v>641</v>
@@ -3734,13 +3763,13 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>517</v>
-      </c>
-      <c r="C59" s="20" t="s">
-        <v>243</v>
+        <v>516</v>
+      </c>
+      <c r="C59" s="16" t="s">
+        <v>641</v>
       </c>
       <c r="D59" s="20"/>
       <c r="E59" s="20"/>
@@ -3751,13 +3780,13 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
-        <v>327</v>
+        <v>515</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>384</v>
+        <v>517</v>
       </c>
       <c r="C60" s="20" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="D60" s="20"/>
       <c r="E60" s="20"/>
@@ -3768,13 +3797,13 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C61" s="20" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D61" s="20"/>
       <c r="E61" s="20"/>
@@ -3785,13 +3814,13 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C62" s="20" t="s">
-        <v>356</v>
+        <v>239</v>
       </c>
       <c r="D62" s="20"/>
       <c r="E62" s="20"/>
@@ -3802,13 +3831,13 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B63" s="11" t="s">
-        <v>387</v>
+        <v>329</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>386</v>
       </c>
       <c r="C63" s="20" t="s">
-        <v>240</v>
+        <v>356</v>
       </c>
       <c r="D63" s="20"/>
       <c r="E63" s="20"/>
@@ -3819,13 +3848,13 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C64" s="20" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D64" s="20"/>
       <c r="E64" s="20"/>
@@ -3836,13 +3865,13 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C65" s="20" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D65" s="20"/>
       <c r="E65" s="20"/>
@@ -3853,13 +3882,13 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C66" s="20" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D66" s="20"/>
       <c r="E66" s="20"/>
@@ -3870,10 +3899,10 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C67" s="20" t="s">
         <v>239</v>
@@ -3887,13 +3916,13 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
-        <v>330</v>
-      </c>
-      <c r="B68" s="10" t="s">
-        <v>392</v>
-      </c>
-      <c r="C68" s="16" t="s">
-        <v>641</v>
+        <v>23</v>
+      </c>
+      <c r="B68" s="11" t="s">
+        <v>391</v>
+      </c>
+      <c r="C68" s="20" t="s">
+        <v>239</v>
       </c>
       <c r="D68" s="20"/>
       <c r="E68" s="20"/>
@@ -3904,13 +3933,13 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B69" s="10" t="s">
-        <v>393</v>
-      </c>
-      <c r="C69" s="20" t="s">
-        <v>243</v>
+        <v>392</v>
+      </c>
+      <c r="C69" s="16" t="s">
+        <v>641</v>
       </c>
       <c r="D69" s="20"/>
       <c r="E69" s="20"/>
@@ -3921,13 +3950,13 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B70" s="11" t="s">
-        <v>394</v>
+        <v>331</v>
+      </c>
+      <c r="B70" s="10" t="s">
+        <v>393</v>
       </c>
       <c r="C70" s="20" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="D70" s="20"/>
       <c r="E70" s="20"/>
@@ -3938,13 +3967,13 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C71" s="20" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D71" s="20"/>
       <c r="E71" s="20"/>
@@ -3955,13 +3984,13 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
-        <v>332</v>
-      </c>
-      <c r="B72" s="10" t="s">
-        <v>396</v>
+        <v>47</v>
+      </c>
+      <c r="B72" s="11" t="s">
+        <v>395</v>
       </c>
       <c r="C72" s="20" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D72" s="20"/>
       <c r="E72" s="20"/>
@@ -3971,17 +4000,17 @@
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B73" s="7" t="s">
-        <v>397</v>
-      </c>
-      <c r="C73" s="16" t="s">
+      <c r="A73" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="B73" s="10" t="s">
+        <v>396</v>
+      </c>
+      <c r="C73" s="20" t="s">
         <v>239</v>
       </c>
-      <c r="D73" s="16"/>
-      <c r="E73" s="16"/>
+      <c r="D73" s="20"/>
+      <c r="E73" s="20"/>
       <c r="F73" s="9"/>
       <c r="G73" s="1" t="s">
         <v>539</v>
@@ -3989,10 +4018,10 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C74" s="16" t="s">
         <v>239</v>
@@ -4006,10 +4035,10 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
-        <v>333</v>
-      </c>
-      <c r="B75" s="10" t="s">
-        <v>399</v>
+        <v>49</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>398</v>
       </c>
       <c r="C75" s="16" t="s">
         <v>239</v>
@@ -4023,10 +4052,10 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B76" s="7" t="s">
-        <v>400</v>
+        <v>333</v>
+      </c>
+      <c r="B76" s="10" t="s">
+        <v>399</v>
       </c>
       <c r="C76" s="16" t="s">
         <v>239</v>
@@ -4040,13 +4069,13 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C77" s="16" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D77" s="16"/>
       <c r="E77" s="16"/>
@@ -4057,10 +4086,10 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
-        <v>334</v>
-      </c>
-      <c r="B78" s="10" t="s">
-        <v>402</v>
+        <v>51</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>401</v>
       </c>
       <c r="C78" s="16" t="s">
         <v>240</v>
@@ -4074,10 +4103,10 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>657</v>
+        <v>334</v>
+      </c>
+      <c r="B79" s="10" t="s">
+        <v>402</v>
       </c>
       <c r="C79" s="16" t="s">
         <v>240</v>
@@ -4090,14 +4119,14 @@
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="11" t="s">
-        <v>658</v>
+      <c r="A80" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="C80" s="16" t="s">
-        <v>656</v>
+        <v>240</v>
       </c>
       <c r="D80" s="16"/>
       <c r="E80" s="16"/>
@@ -4107,14 +4136,14 @@
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="7" t="s">
-        <v>335</v>
-      </c>
-      <c r="B81" s="10" t="s">
-        <v>403</v>
+      <c r="A81" s="11" t="s">
+        <v>658</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>655</v>
       </c>
       <c r="C81" s="16" t="s">
-        <v>240</v>
+        <v>656</v>
       </c>
       <c r="D81" s="16"/>
       <c r="E81" s="16"/>
@@ -4125,13 +4154,13 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C82" s="16" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D82" s="16"/>
       <c r="E82" s="16"/>
@@ -4142,13 +4171,13 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B83" s="10" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C83" s="16" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D83" s="16"/>
       <c r="E83" s="16"/>
@@ -4159,13 +4188,13 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B84" s="10" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C84" s="16" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D84" s="16"/>
       <c r="E84" s="16"/>
@@ -4176,10 +4205,10 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B85" s="10" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C85" s="16" t="s">
         <v>239</v>
@@ -4193,10 +4222,10 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B86" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C86" s="16" t="s">
         <v>239</v>
@@ -4210,13 +4239,13 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B87" s="7" t="s">
-        <v>192</v>
+        <v>340</v>
+      </c>
+      <c r="B87" s="10" t="s">
+        <v>408</v>
       </c>
       <c r="C87" s="16" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D87" s="16"/>
       <c r="E87" s="16"/>
@@ -4227,10 +4256,10 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C88" s="16" t="s">
         <v>243</v>
@@ -4244,10 +4273,10 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>409</v>
+        <v>193</v>
       </c>
       <c r="C89" s="16" t="s">
         <v>243</v>
@@ -4261,10 +4290,10 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="B90" s="10" t="s">
-        <v>410</v>
+        <v>41</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>409</v>
       </c>
       <c r="C90" s="16" t="s">
         <v>243</v>
@@ -4278,13 +4307,13 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
-        <v>644</v>
+        <v>341</v>
       </c>
       <c r="B91" s="10" t="s">
-        <v>645</v>
+        <v>410</v>
       </c>
       <c r="C91" s="16" t="s">
-        <v>357</v>
+        <v>243</v>
       </c>
       <c r="D91" s="16"/>
       <c r="E91" s="16"/>
@@ -4295,16 +4324,16 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>411</v>
+        <v>644</v>
+      </c>
+      <c r="B92" s="10" t="s">
+        <v>645</v>
       </c>
       <c r="C92" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="D92" s="19"/>
-      <c r="E92" s="19"/>
+        <v>357</v>
+      </c>
+      <c r="D92" s="16"/>
+      <c r="E92" s="16"/>
       <c r="F92" s="9"/>
       <c r="G92" s="1" t="s">
         <v>539</v>
@@ -4312,16 +4341,16 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
-        <v>342</v>
-      </c>
-      <c r="B93" s="10" t="s">
-        <v>412</v>
+        <v>42</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>411</v>
       </c>
       <c r="C93" s="16" t="s">
-        <v>357</v>
-      </c>
-      <c r="D93" s="16"/>
-      <c r="E93" s="16"/>
+        <v>244</v>
+      </c>
+      <c r="D93" s="19"/>
+      <c r="E93" s="19"/>
       <c r="F93" s="9"/>
       <c r="G93" s="1" t="s">
         <v>539</v>
@@ -4329,13 +4358,13 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B94" s="10" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C94" s="16" t="s">
-        <v>242</v>
+        <v>357</v>
       </c>
       <c r="D94" s="16"/>
       <c r="E94" s="16"/>
@@ -4345,14 +4374,14 @@
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="9" t="s">
-        <v>519</v>
+      <c r="A95" s="7" t="s">
+        <v>343</v>
       </c>
       <c r="B95" s="10" t="s">
-        <v>509</v>
+        <v>413</v>
       </c>
       <c r="C95" s="16" t="s">
-        <v>642</v>
+        <v>242</v>
       </c>
       <c r="D95" s="16"/>
       <c r="E95" s="16"/>
@@ -4363,13 +4392,13 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
-        <v>510</v>
+        <v>519</v>
       </c>
       <c r="B96" s="10" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="C96" s="16" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="D96" s="16"/>
       <c r="E96" s="16"/>
@@ -4380,10 +4409,10 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="9" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B97" s="10" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="C97" s="16" t="s">
         <v>643</v>
@@ -4397,13 +4426,13 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
-        <v>648</v>
+        <v>511</v>
       </c>
       <c r="B98" s="10" t="s">
-        <v>640</v>
+        <v>512</v>
       </c>
       <c r="C98" s="16" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="D98" s="16"/>
       <c r="E98" s="16"/>
@@ -4413,45 +4442,45 @@
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B99" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="C99" s="21" t="s">
-        <v>254</v>
+      <c r="A99" s="9" t="s">
+        <v>648</v>
+      </c>
+      <c r="B99" s="10" t="s">
+        <v>640</v>
+      </c>
+      <c r="C99" s="16" t="s">
+        <v>641</v>
       </c>
       <c r="D99" s="16"/>
       <c r="E99" s="16"/>
-      <c r="F99" s="7"/>
+      <c r="F99" s="9"/>
       <c r="G99" s="1" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>414</v>
+        <v>250</v>
       </c>
       <c r="C100" s="21" t="s">
         <v>254</v>
       </c>
       <c r="D100" s="16"/>
       <c r="E100" s="16"/>
-      <c r="F100" s="9"/>
+      <c r="F100" s="7"/>
       <c r="G100" s="1" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B101" s="9" t="s">
-        <v>415</v>
+        <v>44</v>
+      </c>
+      <c r="B101" s="7" t="s">
+        <v>414</v>
       </c>
       <c r="C101" s="21" t="s">
         <v>254</v>
@@ -4465,44 +4494,44 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="7" t="s">
-        <v>134</v>
+        <v>45</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>249</v>
+        <v>415</v>
       </c>
       <c r="C102" s="21" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D102" s="16"/>
       <c r="E102" s="16"/>
-      <c r="F102" s="7"/>
+      <c r="F102" s="9"/>
       <c r="G102" s="1" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>416</v>
+        <v>249</v>
       </c>
       <c r="C103" s="21" t="s">
         <v>255</v>
       </c>
       <c r="D103" s="16"/>
       <c r="E103" s="16"/>
-      <c r="F103" s="9"/>
+      <c r="F103" s="7"/>
       <c r="G103" s="1" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="B104" s="7" t="s">
-        <v>417</v>
+        <v>135</v>
+      </c>
+      <c r="B104" s="9" t="s">
+        <v>416</v>
       </c>
       <c r="C104" s="21" t="s">
         <v>255</v>
@@ -4516,13 +4545,13 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C105" s="21" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D105" s="16"/>
       <c r="E105" s="16"/>
@@ -4533,13 +4562,13 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>251</v>
+        <v>418</v>
       </c>
       <c r="C106" s="21" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="D106" s="16"/>
       <c r="E106" s="16"/>
@@ -4550,17 +4579,15 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>419</v>
+        <v>251</v>
       </c>
       <c r="C107" s="21" t="s">
-        <v>268</v>
-      </c>
-      <c r="D107" s="16" t="s">
-        <v>257</v>
-      </c>
+        <v>254</v>
+      </c>
+      <c r="D107" s="16"/>
       <c r="E107" s="16"/>
       <c r="F107" s="9"/>
       <c r="G107" s="1" t="s">
@@ -4569,10 +4596,10 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C108" s="21" t="s">
         <v>268</v>
@@ -4588,15 +4615,17 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>253</v>
+        <v>420</v>
       </c>
       <c r="C109" s="21" t="s">
-        <v>255</v>
-      </c>
-      <c r="D109" s="16"/>
+        <v>268</v>
+      </c>
+      <c r="D109" s="16" t="s">
+        <v>257</v>
+      </c>
       <c r="E109" s="16"/>
       <c r="F109" s="9"/>
       <c r="G109" s="1" t="s">
@@ -4605,17 +4634,15 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>421</v>
+        <v>253</v>
       </c>
       <c r="C110" s="21" t="s">
         <v>255</v>
       </c>
-      <c r="D110" s="16" t="s">
-        <v>257</v>
-      </c>
+      <c r="D110" s="16"/>
       <c r="E110" s="16"/>
       <c r="F110" s="9"/>
       <c r="G110" s="1" t="s">
@@ -4624,15 +4651,17 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C111" s="21" t="s">
         <v>255</v>
       </c>
-      <c r="D111" s="16"/>
+      <c r="D111" s="16" t="s">
+        <v>257</v>
+      </c>
       <c r="E111" s="16"/>
       <c r="F111" s="9"/>
       <c r="G111" s="1" t="s">
@@ -4641,13 +4670,13 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C112" s="21" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="D112" s="16"/>
       <c r="E112" s="16"/>
@@ -4658,13 +4687,13 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="7" t="s">
-        <v>344</v>
-      </c>
-      <c r="B113" s="10" t="s">
-        <v>424</v>
-      </c>
-      <c r="C113" s="16" t="s">
-        <v>641</v>
+        <v>144</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="C113" s="21" t="s">
+        <v>252</v>
       </c>
       <c r="D113" s="16"/>
       <c r="E113" s="16"/>
@@ -4675,13 +4704,13 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
-        <v>306</v>
-      </c>
-      <c r="B114" s="9" t="s">
-        <v>308</v>
-      </c>
-      <c r="C114" s="21" t="s">
-        <v>310</v>
+        <v>344</v>
+      </c>
+      <c r="B114" s="10" t="s">
+        <v>424</v>
+      </c>
+      <c r="C114" s="16" t="s">
+        <v>641</v>
       </c>
       <c r="D114" s="16"/>
       <c r="E114" s="16"/>
@@ -4692,13 +4721,13 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B115" s="9" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C115" s="21" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D115" s="16"/>
       <c r="E115" s="16"/>
@@ -4709,35 +4738,33 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="B116" s="9" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C116" s="21" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D116" s="16"/>
       <c r="E116" s="16"/>
-      <c r="F116" s="7"/>
+      <c r="F116" s="9"/>
       <c r="G116" s="1" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A117" s="9" t="s">
-        <v>145</v>
+      <c r="A117" s="7" t="s">
+        <v>312</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>194</v>
+        <v>313</v>
       </c>
       <c r="C117" s="21" t="s">
-        <v>205</v>
+        <v>314</v>
       </c>
       <c r="D117" s="16"/>
-      <c r="E117" s="16" t="s">
-        <v>257</v>
-      </c>
+      <c r="E117" s="16"/>
       <c r="F117" s="7"/>
       <c r="G117" s="1" t="s">
         <v>539</v>
@@ -4745,16 +4772,16 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="B118" s="7" t="s">
-        <v>195</v>
+        <v>145</v>
+      </c>
+      <c r="B118" s="9" t="s">
+        <v>194</v>
       </c>
       <c r="C118" s="21" t="s">
         <v>205</v>
       </c>
-      <c r="D118" s="15"/>
-      <c r="E118" s="15" t="s">
+      <c r="D118" s="16"/>
+      <c r="E118" s="16" t="s">
         <v>257</v>
       </c>
       <c r="F118" s="7"/>
@@ -4763,11 +4790,11 @@
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A119" s="7" t="s">
-        <v>147</v>
+      <c r="A119" s="9" t="s">
+        <v>146</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C119" s="21" t="s">
         <v>205</v>
@@ -4782,11 +4809,11 @@
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A120" s="9" t="s">
-        <v>148</v>
+      <c r="A120" s="7" t="s">
+        <v>147</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C120" s="21" t="s">
         <v>205</v>
@@ -4801,11 +4828,11 @@
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A121" s="7" t="s">
-        <v>149</v>
+      <c r="A121" s="9" t="s">
+        <v>148</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>425</v>
+        <v>198</v>
       </c>
       <c r="C121" s="21" t="s">
         <v>205</v>
@@ -4814,17 +4841,17 @@
       <c r="E121" s="15" t="s">
         <v>257</v>
       </c>
-      <c r="F121" s="9"/>
+      <c r="F121" s="7"/>
       <c r="G121" s="1" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A122" s="9" t="s">
-        <v>150</v>
+      <c r="A122" s="7" t="s">
+        <v>149</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C122" s="21" t="s">
         <v>205</v>
@@ -4840,10 +4867,10 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C123" s="21" t="s">
         <v>205</v>
@@ -4858,11 +4885,11 @@
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A124" s="7" t="s">
-        <v>152</v>
+      <c r="A124" s="9" t="s">
+        <v>151</v>
       </c>
       <c r="B124" s="7" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C124" s="21" t="s">
         <v>205</v>
@@ -4877,11 +4904,11 @@
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A125" s="9" t="s">
-        <v>153</v>
+      <c r="A125" s="7" t="s">
+        <v>152</v>
       </c>
       <c r="B125" s="7" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C125" s="21" t="s">
         <v>205</v>
@@ -4896,11 +4923,11 @@
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A126" s="7" t="s">
-        <v>154</v>
+      <c r="A126" s="9" t="s">
+        <v>153</v>
       </c>
       <c r="B126" s="7" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C126" s="21" t="s">
         <v>205</v>
@@ -4915,11 +4942,11 @@
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A127" s="9" t="s">
-        <v>155</v>
+      <c r="A127" s="7" t="s">
+        <v>154</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C127" s="21" t="s">
         <v>205</v>
@@ -4935,10 +4962,10 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="B128" s="9" t="s">
-        <v>432</v>
+        <v>155</v>
+      </c>
+      <c r="B128" s="7" t="s">
+        <v>431</v>
       </c>
       <c r="C128" s="21" t="s">
         <v>205</v>
@@ -4953,17 +4980,19 @@
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A129" s="7" t="s">
-        <v>53</v>
+      <c r="A129" s="9" t="s">
+        <v>156</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>220</v>
+        <v>432</v>
       </c>
       <c r="C129" s="21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D129" s="15"/>
-      <c r="E129" s="15"/>
+      <c r="E129" s="15" t="s">
+        <v>257</v>
+      </c>
       <c r="F129" s="9"/>
       <c r="G129" s="1" t="s">
         <v>539</v>
@@ -4971,10 +5000,10 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="7" t="s">
-        <v>646</v>
+        <v>53</v>
       </c>
       <c r="B130" s="9" t="s">
-        <v>647</v>
+        <v>220</v>
       </c>
       <c r="C130" s="21" t="s">
         <v>206</v>
@@ -4987,11 +5016,11 @@
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A131" s="9" t="s">
-        <v>54</v>
+      <c r="A131" s="7" t="s">
+        <v>646</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>221</v>
+        <v>647</v>
       </c>
       <c r="C131" s="21" t="s">
         <v>206</v>
@@ -5004,11 +5033,11 @@
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A132" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="B132" s="10" t="s">
-        <v>433</v>
+      <c r="A132" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B132" s="9" t="s">
+        <v>221</v>
       </c>
       <c r="C132" s="21" t="s">
         <v>206</v>
@@ -5022,10 +5051,10 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="7" t="s">
-        <v>633</v>
+        <v>345</v>
       </c>
       <c r="B133" s="10" t="s">
-        <v>634</v>
+        <v>433</v>
       </c>
       <c r="C133" s="21" t="s">
         <v>206</v>
@@ -5039,10 +5068,10 @@
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="7" t="s">
-        <v>346</v>
+        <v>633</v>
       </c>
       <c r="B134" s="10" t="s">
-        <v>434</v>
+        <v>634</v>
       </c>
       <c r="C134" s="21" t="s">
         <v>206</v>
@@ -5056,10 +5085,10 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="7" t="s">
-        <v>653</v>
+        <v>346</v>
       </c>
       <c r="B135" s="10" t="s">
-        <v>654</v>
+        <v>434</v>
       </c>
       <c r="C135" s="21" t="s">
         <v>206</v>
@@ -5073,10 +5102,10 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="7" t="s">
-        <v>347</v>
+        <v>653</v>
       </c>
       <c r="B136" s="10" t="s">
-        <v>435</v>
+        <v>654</v>
       </c>
       <c r="C136" s="21" t="s">
         <v>206</v>
@@ -5090,10 +5119,10 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="7" t="s">
-        <v>635</v>
+        <v>347</v>
       </c>
       <c r="B137" s="10" t="s">
-        <v>636</v>
+        <v>435</v>
       </c>
       <c r="C137" s="21" t="s">
         <v>206</v>
@@ -5107,10 +5136,10 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="7" t="s">
-        <v>348</v>
+        <v>635</v>
       </c>
       <c r="B138" s="10" t="s">
-        <v>436</v>
+        <v>636</v>
       </c>
       <c r="C138" s="21" t="s">
         <v>206</v>
@@ -5124,13 +5153,13 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
-        <v>637</v>
-      </c>
-      <c r="B139" s="9" t="s">
-        <v>638</v>
+        <v>348</v>
+      </c>
+      <c r="B139" s="10" t="s">
+        <v>436</v>
       </c>
       <c r="C139" s="21" t="s">
-        <v>639</v>
+        <v>206</v>
       </c>
       <c r="D139" s="15"/>
       <c r="E139" s="15"/>
@@ -5141,13 +5170,13 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="7" t="s">
-        <v>349</v>
-      </c>
-      <c r="B140" s="10" t="s">
-        <v>364</v>
+        <v>637</v>
+      </c>
+      <c r="B140" s="9" t="s">
+        <v>638</v>
       </c>
       <c r="C140" s="21" t="s">
-        <v>206</v>
+        <v>639</v>
       </c>
       <c r="D140" s="15"/>
       <c r="E140" s="15"/>
@@ -5158,10 +5187,10 @@
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B141" s="10" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C141" s="21" t="s">
         <v>206</v>
@@ -5175,10 +5204,10 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="7" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B142" s="10" t="s">
-        <v>437</v>
+        <v>365</v>
       </c>
       <c r="C142" s="21" t="s">
         <v>206</v>
@@ -5192,10 +5221,10 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="7" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B143" s="10" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C143" s="21" t="s">
         <v>206</v>
@@ -5209,10 +5238,10 @@
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="7" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B144" s="10" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C144" s="21" t="s">
         <v>206</v>
@@ -5226,12 +5255,12 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="7" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B145" s="10" t="s">
-        <v>440</v>
-      </c>
-      <c r="C145" s="15" t="s">
+        <v>439</v>
+      </c>
+      <c r="C145" s="21" t="s">
         <v>206</v>
       </c>
       <c r="D145" s="15"/>
@@ -5243,13 +5272,13 @@
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="7" t="s">
-        <v>315</v>
-      </c>
-      <c r="B146" s="7" t="s">
-        <v>441</v>
-      </c>
-      <c r="C146" s="16" t="s">
-        <v>522</v>
+        <v>354</v>
+      </c>
+      <c r="B146" s="10" t="s">
+        <v>440</v>
+      </c>
+      <c r="C146" s="15" t="s">
+        <v>206</v>
       </c>
       <c r="D146" s="15"/>
       <c r="E146" s="15"/>
@@ -5260,13 +5289,13 @@
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="7" t="s">
-        <v>55</v>
+        <v>315</v>
       </c>
       <c r="B147" s="7" t="s">
-        <v>210</v>
+        <v>441</v>
       </c>
       <c r="C147" s="16" t="s">
-        <v>207</v>
+        <v>522</v>
       </c>
       <c r="D147" s="15"/>
       <c r="E147" s="15"/>
@@ -5277,10 +5306,10 @@
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B148" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C148" s="16" t="s">
         <v>207</v>
@@ -5294,10 +5323,10 @@
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B149" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C149" s="16" t="s">
         <v>207</v>
@@ -5311,10 +5340,10 @@
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B150" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C150" s="16" t="s">
         <v>207</v>
@@ -5328,10 +5357,10 @@
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B151" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C151" s="16" t="s">
         <v>207</v>
@@ -5345,10 +5374,10 @@
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B152" s="7" t="s">
-        <v>442</v>
+        <v>214</v>
       </c>
       <c r="C152" s="16" t="s">
         <v>207</v>
@@ -5362,10 +5391,10 @@
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B153" s="7" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C153" s="16" t="s">
         <v>207</v>
@@ -5379,10 +5408,10 @@
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B154" s="7" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C154" s="16" t="s">
         <v>207</v>
@@ -5396,10 +5425,10 @@
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B155" s="7" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C155" s="16" t="s">
         <v>207</v>
@@ -5413,10 +5442,10 @@
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B156" s="7" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C156" s="16" t="s">
         <v>207</v>
@@ -5429,11 +5458,11 @@
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A157" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B157" s="9" t="s">
-        <v>447</v>
+      <c r="A157" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B157" s="7" t="s">
+        <v>446</v>
       </c>
       <c r="C157" s="16" t="s">
         <v>207</v>
@@ -5446,11 +5475,11 @@
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A158" s="7" t="s">
-        <v>66</v>
+      <c r="A158" s="9" t="s">
+        <v>65</v>
       </c>
       <c r="B158" s="9" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C158" s="16" t="s">
         <v>207</v>
@@ -5464,10 +5493,10 @@
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B159" s="9" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C159" s="16" t="s">
         <v>207</v>
@@ -5481,10 +5510,10 @@
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B160" s="9" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C160" s="16" t="s">
         <v>207</v>
@@ -5498,10 +5527,10 @@
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B161" s="7" t="s">
-        <v>451</v>
+        <v>68</v>
+      </c>
+      <c r="B161" s="9" t="s">
+        <v>450</v>
       </c>
       <c r="C161" s="16" t="s">
         <v>207</v>
@@ -5515,29 +5544,29 @@
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="B162" s="9" t="s">
-        <v>200</v>
+        <v>69</v>
+      </c>
+      <c r="B162" s="7" t="s">
+        <v>451</v>
       </c>
       <c r="C162" s="16" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D162" s="15"/>
       <c r="E162" s="15"/>
-      <c r="F162" s="7"/>
+      <c r="F162" s="9"/>
       <c r="G162" s="1" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="7" t="s">
-        <v>297</v>
-      </c>
-      <c r="B163" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="C163" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B163" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="C163" s="16" t="s">
         <v>208</v>
       </c>
       <c r="D163" s="15"/>
@@ -5549,27 +5578,27 @@
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C164" s="21" t="s">
         <v>208</v>
       </c>
       <c r="D164" s="15"/>
       <c r="E164" s="15"/>
-      <c r="F164" s="11"/>
+      <c r="F164" s="7"/>
       <c r="G164" s="1" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B165" s="7" t="s">
-        <v>201</v>
+        <v>298</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>203</v>
       </c>
       <c r="C165" s="21" t="s">
         <v>208</v>
@@ -5583,15 +5612,15 @@
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="7" t="s">
-        <v>299</v>
+        <v>71</v>
       </c>
       <c r="B166" s="7" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C166" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="D166" s="16"/>
+      <c r="D166" s="15"/>
       <c r="E166" s="15"/>
       <c r="F166" s="11"/>
       <c r="G166" s="1" t="s">
@@ -5600,32 +5629,32 @@
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="7" t="s">
-        <v>72</v>
+        <v>299</v>
       </c>
       <c r="B167" s="7" t="s">
-        <v>452</v>
+        <v>204</v>
       </c>
       <c r="C167" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="D167" s="15"/>
+      <c r="D167" s="16"/>
       <c r="E167" s="15"/>
-      <c r="F167" s="9"/>
+      <c r="F167" s="11"/>
       <c r="G167" s="1" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="7" t="s">
-        <v>300</v>
+        <v>72</v>
       </c>
       <c r="B168" s="7" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C168" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="D168" s="16"/>
+      <c r="D168" s="15"/>
       <c r="E168" s="15"/>
       <c r="F168" s="9"/>
       <c r="G168" s="1" t="s">
@@ -5634,15 +5663,15 @@
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B169" s="7" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C169" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="D169" s="15"/>
+      <c r="D169" s="16"/>
       <c r="E169" s="15"/>
       <c r="F169" s="9"/>
       <c r="G169" s="1" t="s">
@@ -5651,10 +5680,10 @@
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="7" t="s">
-        <v>73</v>
+        <v>301</v>
       </c>
       <c r="B170" s="7" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C170" s="21" t="s">
         <v>208</v>
@@ -5668,10 +5697,10 @@
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="7" t="s">
-        <v>302</v>
+        <v>73</v>
       </c>
       <c r="B171" s="7" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C171" s="21" t="s">
         <v>208</v>
@@ -5685,10 +5714,10 @@
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="7" t="s">
-        <v>74</v>
+        <v>302</v>
       </c>
       <c r="B172" s="7" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C172" s="21" t="s">
         <v>208</v>
@@ -5702,10 +5731,10 @@
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="7" t="s">
-        <v>303</v>
+        <v>74</v>
       </c>
       <c r="B173" s="7" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C173" s="21" t="s">
         <v>208</v>
@@ -5719,10 +5748,10 @@
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B174" s="7" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C174" s="21" t="s">
         <v>208</v>
@@ -5736,10 +5765,10 @@
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="7" t="s">
-        <v>75</v>
+        <v>304</v>
       </c>
       <c r="B175" s="7" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C175" s="21" t="s">
         <v>208</v>
@@ -5753,10 +5782,10 @@
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" s="7" t="s">
-        <v>305</v>
+        <v>75</v>
       </c>
       <c r="B176" s="7" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C176" s="21" t="s">
         <v>208</v>
@@ -5770,49 +5799,49 @@
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" s="7" t="s">
-        <v>76</v>
+        <v>305</v>
       </c>
       <c r="B177" s="7" t="s">
-        <v>215</v>
+        <v>461</v>
       </c>
       <c r="C177" s="21" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D177" s="15"/>
       <c r="E177" s="15"/>
-      <c r="F177" s="12"/>
+      <c r="F177" s="9"/>
       <c r="G177" s="1" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="B178" s="9" t="s">
-        <v>216</v>
+        <v>76</v>
+      </c>
+      <c r="B178" s="7" t="s">
+        <v>215</v>
       </c>
       <c r="C178" s="21" t="s">
         <v>209</v>
       </c>
       <c r="D178" s="15"/>
       <c r="E178" s="15"/>
-      <c r="F178" s="11"/>
+      <c r="F178" s="12"/>
       <c r="G178" s="1" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B179" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C179" s="21" t="s">
         <v>209</v>
       </c>
-      <c r="D179" s="16"/>
+      <c r="D179" s="15"/>
       <c r="E179" s="15"/>
       <c r="F179" s="11"/>
       <c r="G179" s="1" t="s">
@@ -5821,27 +5850,27 @@
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="B180" s="1" t="s">
-        <v>462</v>
+        <v>78</v>
+      </c>
+      <c r="B180" s="9" t="s">
+        <v>217</v>
       </c>
       <c r="C180" s="21" t="s">
         <v>209</v>
       </c>
-      <c r="D180" s="15"/>
+      <c r="D180" s="16"/>
       <c r="E180" s="15"/>
-      <c r="F180" s="9"/>
+      <c r="F180" s="11"/>
       <c r="G180" s="1" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C181" s="21" t="s">
         <v>209</v>
@@ -5855,10 +5884,10 @@
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B182" s="7" t="s">
-        <v>464</v>
+        <v>80</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>463</v>
       </c>
       <c r="C182" s="21" t="s">
         <v>209</v>
@@ -5872,10 +5901,10 @@
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B183" s="7" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C183" s="21" t="s">
         <v>209</v>
@@ -5889,10 +5918,10 @@
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B184" s="7" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C184" s="21" t="s">
         <v>209</v>
@@ -5906,15 +5935,15 @@
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B185" s="7" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C185" s="21" t="s">
         <v>209</v>
       </c>
-      <c r="D185" s="16"/>
+      <c r="D185" s="15"/>
       <c r="E185" s="15"/>
       <c r="F185" s="9"/>
       <c r="G185" s="1" t="s">
@@ -5923,15 +5952,15 @@
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B186" s="9" t="s">
-        <v>532</v>
+        <v>84</v>
+      </c>
+      <c r="B186" s="7" t="s">
+        <v>467</v>
       </c>
       <c r="C186" s="21" t="s">
-        <v>241</v>
-      </c>
-      <c r="D186" s="15"/>
+        <v>209</v>
+      </c>
+      <c r="D186" s="16"/>
       <c r="E186" s="15"/>
       <c r="F186" s="9"/>
       <c r="G186" s="1" t="s">
@@ -5940,13 +5969,13 @@
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="B187" s="7" t="s">
-        <v>468</v>
+        <v>85</v>
+      </c>
+      <c r="B187" s="9" t="s">
+        <v>532</v>
       </c>
       <c r="C187" s="21" t="s">
-        <v>265</v>
+        <v>241</v>
       </c>
       <c r="D187" s="15"/>
       <c r="E187" s="15"/>
@@ -5957,10 +5986,10 @@
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B188" s="7" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C188" s="21" t="s">
         <v>265</v>
@@ -5974,10 +6003,10 @@
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B189" s="7" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C189" s="21" t="s">
         <v>265</v>
@@ -5991,10 +6020,10 @@
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B190" s="7" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C190" s="21" t="s">
         <v>265</v>
@@ -6008,10 +6037,10 @@
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B191" s="7" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C191" s="21" t="s">
         <v>265</v>
@@ -6025,10 +6054,10 @@
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B192" s="7" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C192" s="21" t="s">
         <v>265</v>
@@ -6042,15 +6071,15 @@
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B193" s="7" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C193" s="21" t="s">
         <v>265</v>
       </c>
-      <c r="D193" s="16"/>
+      <c r="D193" s="15"/>
       <c r="E193" s="15"/>
       <c r="F193" s="9"/>
       <c r="G193" s="1" t="s">
@@ -6059,15 +6088,15 @@
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B194" s="7" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C194" s="21" t="s">
         <v>265</v>
       </c>
-      <c r="D194" s="15"/>
+      <c r="D194" s="16"/>
       <c r="E194" s="15"/>
       <c r="F194" s="9"/>
       <c r="G194" s="1" t="s">
@@ -6076,10 +6105,10 @@
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="B195" s="9" t="s">
-        <v>476</v>
+        <v>164</v>
+      </c>
+      <c r="B195" s="7" t="s">
+        <v>475</v>
       </c>
       <c r="C195" s="21" t="s">
         <v>265</v>
@@ -6093,13 +6122,13 @@
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="B196" s="1" t="s">
-        <v>218</v>
+        <v>165</v>
+      </c>
+      <c r="B196" s="9" t="s">
+        <v>476</v>
       </c>
       <c r="C196" s="21" t="s">
-        <v>248</v>
+        <v>265</v>
       </c>
       <c r="D196" s="15"/>
       <c r="E196" s="15"/>
@@ -6110,49 +6139,49 @@
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197" s="7" t="s">
-        <v>630</v>
+        <v>86</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>629</v>
+        <v>218</v>
       </c>
       <c r="C197" s="21" t="s">
         <v>248</v>
       </c>
       <c r="D197" s="15"/>
       <c r="E197" s="15"/>
-      <c r="F197" s="9" t="s">
-        <v>631</v>
-      </c>
+      <c r="F197" s="9"/>
       <c r="G197" s="1" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" s="7" t="s">
-        <v>87</v>
+        <v>630</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>219</v>
+        <v>629</v>
       </c>
       <c r="C198" s="21" t="s">
-        <v>206</v>
+        <v>248</v>
       </c>
       <c r="D198" s="15"/>
       <c r="E198" s="15"/>
-      <c r="F198" s="9"/>
+      <c r="F198" s="9" t="s">
+        <v>631</v>
+      </c>
       <c r="G198" s="1" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A199" s="9" t="s">
-        <v>520</v>
+      <c r="A199" s="7" t="s">
+        <v>87</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>521</v>
+        <v>219</v>
       </c>
       <c r="C199" s="21" t="s">
-        <v>522</v>
+        <v>206</v>
       </c>
       <c r="D199" s="15"/>
       <c r="E199" s="15"/>
@@ -6162,14 +6191,14 @@
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A200" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="B200" s="9" t="s">
-        <v>527</v>
+      <c r="A200" s="9" t="s">
+        <v>520</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>521</v>
       </c>
       <c r="C200" s="21" t="s">
-        <v>248</v>
+        <v>522</v>
       </c>
       <c r="D200" s="15"/>
       <c r="E200" s="15"/>
@@ -6180,10 +6209,10 @@
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B201" s="9" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C201" s="21" t="s">
         <v>248</v>
@@ -6197,10 +6226,10 @@
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B202" s="9" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C202" s="21" t="s">
         <v>248</v>
@@ -6214,13 +6243,13 @@
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A203" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B203" s="9" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="C203" s="21" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="D203" s="15"/>
       <c r="E203" s="15"/>
@@ -6230,11 +6259,11 @@
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A204" s="9" t="s">
-        <v>524</v>
+      <c r="A204" s="7" t="s">
+        <v>91</v>
       </c>
       <c r="B204" s="9" t="s">
-        <v>534</v>
+        <v>526</v>
       </c>
       <c r="C204" s="21" t="s">
         <v>241</v>
@@ -6248,10 +6277,10 @@
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205" s="9" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B205" s="9" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="C205" s="21" t="s">
         <v>241</v>
@@ -6264,14 +6293,14 @@
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A206" s="7" t="s">
-        <v>92</v>
+      <c r="A206" s="9" t="s">
+        <v>523</v>
       </c>
       <c r="B206" s="9" t="s">
-        <v>525</v>
+        <v>533</v>
       </c>
       <c r="C206" s="21" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="D206" s="15"/>
       <c r="E206" s="15"/>
@@ -6282,25 +6311,27 @@
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207" s="7" t="s">
-        <v>580</v>
+        <v>92</v>
       </c>
       <c r="B207" s="9" t="s">
-        <v>604</v>
+        <v>525</v>
       </c>
       <c r="C207" s="21" t="s">
-        <v>628</v>
+        <v>248</v>
       </c>
       <c r="D207" s="15"/>
       <c r="E207" s="15"/>
       <c r="F207" s="9"/>
-      <c r="G207" s="1"/>
+      <c r="G207" s="1" t="s">
+        <v>539</v>
+      </c>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A208" s="7" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B208" s="9" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C208" s="21" t="s">
         <v>628</v>
@@ -6312,10 +6343,10 @@
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209" s="7" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B209" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C209" s="21" t="s">
         <v>628</v>
@@ -6327,10 +6358,10 @@
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210" s="7" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B210" s="9" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C210" s="21" t="s">
         <v>628</v>
@@ -6342,10 +6373,10 @@
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211" s="7" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B211" s="9" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C211" s="21" t="s">
         <v>628</v>
@@ -6357,10 +6388,10 @@
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A212" s="7" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B212" s="9" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C212" s="21" t="s">
         <v>628</v>
@@ -6372,10 +6403,10 @@
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A213" s="7" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B213" s="9" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C213" s="21" t="s">
         <v>628</v>
@@ -6387,10 +6418,10 @@
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214" s="7" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B214" s="9" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="C214" s="21" t="s">
         <v>628</v>
@@ -6402,10 +6433,10 @@
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215" s="7" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B215" s="9" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C215" s="21" t="s">
         <v>628</v>
@@ -6417,10 +6448,10 @@
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216" s="7" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B216" s="9" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="C216" s="21" t="s">
         <v>628</v>
@@ -6432,10 +6463,10 @@
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217" s="7" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B217" s="9" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="C217" s="21" t="s">
         <v>628</v>
@@ -6447,10 +6478,10 @@
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A218" s="7" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B218" s="9" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="C218" s="21" t="s">
         <v>628</v>
@@ -6462,10 +6493,10 @@
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A219" s="7" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B219" s="9" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C219" s="21" t="s">
         <v>628</v>
@@ -6477,10 +6508,10 @@
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220" s="7" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B220" s="9" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C220" s="21" t="s">
         <v>628</v>
@@ -6492,10 +6523,10 @@
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A221" s="7" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B221" s="9" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C221" s="21" t="s">
         <v>628</v>
@@ -6507,10 +6538,10 @@
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A222" s="7" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B222" s="9" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C222" s="21" t="s">
         <v>628</v>
@@ -6522,10 +6553,10 @@
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A223" s="7" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B223" s="9" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C223" s="21" t="s">
         <v>628</v>
@@ -6537,10 +6568,10 @@
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224" s="7" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B224" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C224" s="21" t="s">
         <v>628</v>
@@ -6552,10 +6583,10 @@
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B225" s="9" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C225" s="21" t="s">
         <v>628</v>
@@ -6567,10 +6598,10 @@
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226" s="7" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B226" s="9" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C226" s="21" t="s">
         <v>628</v>
@@ -6582,10 +6613,10 @@
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227" s="7" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B227" s="9" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C227" s="21" t="s">
         <v>628</v>
@@ -6597,10 +6628,10 @@
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228" s="7" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B228" s="9" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C228" s="21" t="s">
         <v>628</v>
@@ -6612,10 +6643,10 @@
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A229" s="7" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B229" s="9" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C229" s="21" t="s">
         <v>628</v>
@@ -6627,10 +6658,10 @@
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A230" s="7" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B230" s="9" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C230" s="21" t="s">
         <v>628</v>
@@ -6642,27 +6673,25 @@
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A231" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="B231" s="7" t="s">
-        <v>237</v>
+        <v>603</v>
+      </c>
+      <c r="B231" s="9" t="s">
+        <v>627</v>
       </c>
       <c r="C231" s="21" t="s">
-        <v>246</v>
+        <v>628</v>
       </c>
       <c r="D231" s="15"/>
       <c r="E231" s="15"/>
       <c r="F231" s="9"/>
-      <c r="G231" s="1" t="s">
-        <v>539</v>
-      </c>
+      <c r="G231" s="1"/>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A232" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B232" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C232" s="21" t="s">
         <v>246</v>
@@ -6676,10 +6705,10 @@
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233" s="7" t="s">
-        <v>93</v>
+        <v>167</v>
       </c>
       <c r="B233" s="7" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
       <c r="C233" s="21" t="s">
         <v>246</v>
@@ -6693,17 +6722,15 @@
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A234" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B234" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C234" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="D234" s="15" t="s">
-        <v>257</v>
-      </c>
+      <c r="D234" s="15"/>
       <c r="E234" s="15"/>
       <c r="F234" s="9"/>
       <c r="G234" s="1" t="s">
@@ -6712,15 +6739,17 @@
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A235" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B235" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C235" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="D235" s="15"/>
+      <c r="D235" s="15" t="s">
+        <v>257</v>
+      </c>
       <c r="E235" s="15"/>
       <c r="F235" s="9"/>
       <c r="G235" s="1" t="s">
@@ -6729,17 +6758,15 @@
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A236" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B236" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C236" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="D236" s="15" t="s">
-        <v>257</v>
-      </c>
+      <c r="D236" s="15"/>
       <c r="E236" s="15"/>
       <c r="F236" s="9"/>
       <c r="G236" s="1" t="s">
@@ -6748,15 +6775,17 @@
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B237" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C237" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="D237" s="16"/>
+      <c r="D237" s="15" t="s">
+        <v>257</v>
+      </c>
       <c r="E237" s="15"/>
       <c r="F237" s="9"/>
       <c r="G237" s="1" t="s">
@@ -6765,15 +6794,15 @@
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B238" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C238" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="D238" s="15"/>
+      <c r="D238" s="16"/>
       <c r="E238" s="15"/>
       <c r="F238" s="9"/>
       <c r="G238" s="1" t="s">
@@ -6782,10 +6811,10 @@
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B239" s="9" t="s">
-        <v>228</v>
+        <v>98</v>
+      </c>
+      <c r="B239" s="7" t="s">
+        <v>227</v>
       </c>
       <c r="C239" s="21" t="s">
         <v>246</v>
@@ -6799,10 +6828,10 @@
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240" s="7" t="s">
-        <v>168</v>
+        <v>99</v>
       </c>
       <c r="B240" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C240" s="21" t="s">
         <v>246</v>
@@ -6816,10 +6845,10 @@
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A241" s="7" t="s">
-        <v>100</v>
+        <v>168</v>
       </c>
       <c r="B241" s="9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C241" s="21" t="s">
         <v>246</v>
@@ -6833,10 +6862,10 @@
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A242" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B242" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C242" s="21" t="s">
         <v>246</v>
@@ -6850,10 +6879,10 @@
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A243" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B243" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C243" s="21" t="s">
         <v>246</v>
@@ -6867,10 +6896,10 @@
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A244" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B244" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C244" s="21" t="s">
         <v>246</v>
@@ -6884,10 +6913,10 @@
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A245" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B245" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C245" s="21" t="s">
         <v>246</v>
@@ -6901,10 +6930,10 @@
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A246" s="7" t="s">
-        <v>577</v>
+        <v>104</v>
       </c>
       <c r="B246" s="9" t="s">
-        <v>576</v>
+        <v>234</v>
       </c>
       <c r="C246" s="21" t="s">
         <v>246</v>
@@ -6918,13 +6947,13 @@
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A247" s="7" t="s">
-        <v>105</v>
+        <v>577</v>
       </c>
       <c r="B247" s="9" t="s">
-        <v>235</v>
+        <v>576</v>
       </c>
       <c r="C247" s="21" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D247" s="15"/>
       <c r="E247" s="15"/>
@@ -6935,17 +6964,15 @@
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A248" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B248" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C248" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="D248" s="15" t="s">
-        <v>257</v>
-      </c>
+      <c r="D248" s="15"/>
       <c r="E248" s="15"/>
       <c r="F248" s="9"/>
       <c r="G248" s="1" t="s">
@@ -6954,15 +6981,17 @@
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A249" s="7" t="s">
-        <v>169</v>
+        <v>106</v>
       </c>
       <c r="B249" s="9" t="s">
-        <v>477</v>
+        <v>236</v>
       </c>
       <c r="C249" s="21" t="s">
-        <v>246</v>
-      </c>
-      <c r="D249" s="15"/>
+        <v>247</v>
+      </c>
+      <c r="D249" s="15" t="s">
+        <v>257</v>
+      </c>
       <c r="E249" s="15"/>
       <c r="F249" s="9"/>
       <c r="G249" s="1" t="s">
@@ -6971,10 +7000,10 @@
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A250" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B250" s="9" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C250" s="21" t="s">
         <v>246</v>
@@ -6988,10 +7017,10 @@
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A251" s="7" t="s">
-        <v>107</v>
+        <v>170</v>
       </c>
       <c r="B251" s="9" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C251" s="21" t="s">
         <v>246</v>
@@ -7005,10 +7034,10 @@
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A252" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B252" s="9" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C252" s="21" t="s">
         <v>246</v>
@@ -7022,10 +7051,10 @@
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A253" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B253" s="9" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C253" s="21" t="s">
         <v>246</v>
@@ -7039,17 +7068,15 @@
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A254" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B254" s="9" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C254" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="D254" s="15" t="s">
-        <v>257</v>
-      </c>
+      <c r="D254" s="15"/>
       <c r="E254" s="15"/>
       <c r="F254" s="9"/>
       <c r="G254" s="1" t="s">
@@ -7058,15 +7085,17 @@
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A255" s="7" t="s">
-        <v>171</v>
+        <v>110</v>
       </c>
       <c r="B255" s="9" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C255" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="D255" s="15"/>
+      <c r="D255" s="15" t="s">
+        <v>257</v>
+      </c>
       <c r="E255" s="15"/>
       <c r="F255" s="9"/>
       <c r="G255" s="1" t="s">
@@ -7075,10 +7104,10 @@
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A256" s="7" t="s">
-        <v>111</v>
+        <v>171</v>
       </c>
       <c r="B256" s="9" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C256" s="21" t="s">
         <v>246</v>
@@ -7092,10 +7121,10 @@
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A257" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B257" s="9" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C257" s="21" t="s">
         <v>246</v>
@@ -7109,10 +7138,10 @@
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A258" s="7" t="s">
-        <v>172</v>
+        <v>112</v>
       </c>
       <c r="B258" s="9" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C258" s="21" t="s">
         <v>246</v>
@@ -7126,10 +7155,10 @@
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A259" s="7" t="s">
-        <v>113</v>
+        <v>172</v>
       </c>
       <c r="B259" s="9" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C259" s="21" t="s">
         <v>246</v>
@@ -7143,10 +7172,10 @@
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A260" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B260" s="9" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C260" s="21" t="s">
         <v>246</v>
@@ -7160,10 +7189,10 @@
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A261" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B261" s="9" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C261" s="21" t="s">
         <v>246</v>
@@ -7177,17 +7206,15 @@
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A262" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B262" s="9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C262" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="D262" s="15" t="s">
-        <v>257</v>
-      </c>
+      <c r="D262" s="15"/>
       <c r="E262" s="15"/>
       <c r="F262" s="9"/>
       <c r="G262" s="1" t="s">
@@ -7196,15 +7223,17 @@
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A263" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B263" s="9" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C263" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="D263" s="15"/>
+      <c r="D263" s="15" t="s">
+        <v>257</v>
+      </c>
       <c r="E263" s="15"/>
       <c r="F263" s="9"/>
       <c r="G263" s="1" t="s">
@@ -7213,10 +7242,10 @@
     </row>
     <row r="264" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A264" s="7" t="s">
-        <v>575</v>
+        <v>117</v>
       </c>
       <c r="B264" s="9" t="s">
-        <v>574</v>
+        <v>491</v>
       </c>
       <c r="C264" s="21" t="s">
         <v>246</v>
@@ -7230,13 +7259,13 @@
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A265" s="7" t="s">
-        <v>118</v>
+        <v>575</v>
       </c>
       <c r="B265" s="9" t="s">
-        <v>492</v>
+        <v>574</v>
       </c>
       <c r="C265" s="21" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D265" s="15"/>
       <c r="E265" s="15"/>
@@ -7247,13 +7276,13 @@
     </row>
     <row r="266" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A266" s="7" t="s">
-        <v>173</v>
+        <v>118</v>
       </c>
       <c r="B266" s="9" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C266" s="21" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D266" s="15"/>
       <c r="E266" s="15"/>
@@ -7264,10 +7293,10 @@
     </row>
     <row r="267" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A267" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B267" s="9" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C267" s="21" t="s">
         <v>246</v>
@@ -7281,10 +7310,10 @@
     </row>
     <row r="268" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A268" s="7" t="s">
-        <v>119</v>
+        <v>174</v>
       </c>
       <c r="B268" s="9" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C268" s="21" t="s">
         <v>246</v>
@@ -7298,10 +7327,10 @@
     </row>
     <row r="269" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A269" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B269" s="9" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C269" s="21" t="s">
         <v>246</v>
@@ -7315,10 +7344,10 @@
     </row>
     <row r="270" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A270" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B270" s="9" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C270" s="21" t="s">
         <v>246</v>
@@ -7332,10 +7361,10 @@
     </row>
     <row r="271" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A271" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B271" s="9" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C271" s="21" t="s">
         <v>246</v>
@@ -7349,10 +7378,10 @@
     </row>
     <row r="272" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A272" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B272" s="9" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C272" s="21" t="s">
         <v>246</v>
@@ -7366,10 +7395,10 @@
     </row>
     <row r="273" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A273" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B273" s="9" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C273" s="21" t="s">
         <v>246</v>
@@ -7383,10 +7412,10 @@
     </row>
     <row r="274" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A274" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B274" s="9" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C274" s="21" t="s">
         <v>246</v>
@@ -7400,10 +7429,10 @@
     </row>
     <row r="275" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A275" s="7" t="s">
-        <v>175</v>
+        <v>125</v>
       </c>
       <c r="B275" s="9" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C275" s="21" t="s">
         <v>246</v>
@@ -7417,10 +7446,10 @@
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A276" s="7" t="s">
-        <v>126</v>
+        <v>175</v>
       </c>
       <c r="B276" s="9" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C276" s="21" t="s">
         <v>246</v>
@@ -7434,10 +7463,10 @@
     </row>
     <row r="277" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A277" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B277" s="9" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C277" s="21" t="s">
         <v>246</v>
@@ -7451,10 +7480,10 @@
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A278" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B278" s="9" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C278" s="21" t="s">
         <v>246</v>
@@ -7468,17 +7497,15 @@
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A279" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B279" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C279" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="D279" s="15" t="s">
-        <v>257</v>
-      </c>
+      <c r="D279" s="15"/>
       <c r="E279" s="15"/>
       <c r="F279" s="9"/>
       <c r="G279" s="1" t="s">
@@ -7487,15 +7514,17 @@
     </row>
     <row r="280" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A280" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B280" s="9" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C280" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="D280" s="15"/>
+      <c r="D280" s="15" t="s">
+        <v>257</v>
+      </c>
       <c r="E280" s="15"/>
       <c r="F280" s="9"/>
       <c r="G280" s="1" t="s">
@@ -7504,10 +7533,10 @@
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A281" s="7" t="s">
-        <v>572</v>
+        <v>130</v>
       </c>
       <c r="B281" s="9" t="s">
-        <v>573</v>
+        <v>507</v>
       </c>
       <c r="C281" s="21" t="s">
         <v>246</v>
@@ -7521,13 +7550,13 @@
     </row>
     <row r="282" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A282" s="7" t="s">
-        <v>131</v>
+        <v>572</v>
       </c>
       <c r="B282" s="9" t="s">
-        <v>508</v>
+        <v>573</v>
       </c>
       <c r="C282" s="21" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D282" s="15"/>
       <c r="E282" s="15"/>
@@ -7538,30 +7567,30 @@
     </row>
     <row r="283" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A283" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B283" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="C283" s="16" t="s">
-        <v>566</v>
+        <v>131</v>
+      </c>
+      <c r="B283" s="9" t="s">
+        <v>508</v>
+      </c>
+      <c r="C283" s="21" t="s">
+        <v>247</v>
       </c>
       <c r="D283" s="15"/>
       <c r="E283" s="15"/>
-      <c r="F283" s="15"/>
+      <c r="F283" s="9"/>
       <c r="G283" s="1" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
     </row>
     <row r="284" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A284" s="7" t="s">
-        <v>543</v>
-      </c>
-      <c r="B284" s="9" t="s">
-        <v>548</v>
+        <v>1</v>
+      </c>
+      <c r="B284" s="1" t="s">
+        <v>260</v>
       </c>
       <c r="C284" s="16" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D284" s="15"/>
       <c r="E284" s="15"/>
@@ -7572,13 +7601,13 @@
     </row>
     <row r="285" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A285" s="7" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B285" s="9" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="C285" s="16" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D285" s="15"/>
       <c r="E285" s="15"/>
@@ -7589,13 +7618,13 @@
     </row>
     <row r="286" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A286" s="7" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B286" s="9" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="C286" s="16" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="D286" s="15"/>
       <c r="E286" s="15"/>
@@ -7605,14 +7634,14 @@
       </c>
     </row>
     <row r="287" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A287" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B287" s="7" t="s">
-        <v>178</v>
+      <c r="A287" s="7" t="s">
+        <v>545</v>
+      </c>
+      <c r="B287" s="9" t="s">
+        <v>549</v>
       </c>
       <c r="C287" s="16" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D287" s="15"/>
       <c r="E287" s="15"/>
@@ -7623,13 +7652,13 @@
     </row>
     <row r="288" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A288" s="9" t="s">
-        <v>570</v>
-      </c>
-      <c r="B288" s="9" t="s">
-        <v>571</v>
+        <v>0</v>
+      </c>
+      <c r="B288" s="7" t="s">
+        <v>178</v>
       </c>
       <c r="C288" s="16" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="D288" s="15"/>
       <c r="E288" s="15"/>
@@ -7639,14 +7668,14 @@
       </c>
     </row>
     <row r="289" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A289" s="7" t="s">
-        <v>546</v>
+      <c r="A289" s="9" t="s">
+        <v>570</v>
       </c>
       <c r="B289" s="9" t="s">
-        <v>551</v>
+        <v>571</v>
       </c>
       <c r="C289" s="16" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="D289" s="15"/>
       <c r="E289" s="15"/>
@@ -7657,13 +7686,13 @@
     </row>
     <row r="290" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A290" s="7" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B290" s="9" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C290" s="16" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="D290" s="15"/>
       <c r="E290" s="15"/>
@@ -7674,10 +7703,10 @@
     </row>
     <row r="291" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A291" s="7" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
       <c r="B291" s="9" t="s">
-        <v>560</v>
+        <v>552</v>
       </c>
       <c r="C291" s="16" t="s">
         <v>565</v>
@@ -7691,10 +7720,10 @@
     </row>
     <row r="292" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A292" s="7" t="s">
-        <v>346</v>
+        <v>553</v>
       </c>
       <c r="B292" s="9" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C292" s="16" t="s">
         <v>565</v>
@@ -7708,13 +7737,13 @@
     </row>
     <row r="293" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A293" s="7" t="s">
-        <v>554</v>
+        <v>346</v>
       </c>
       <c r="B293" s="9" t="s">
-        <v>557</v>
+        <v>561</v>
       </c>
       <c r="C293" s="16" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="D293" s="15"/>
       <c r="E293" s="15"/>
@@ -7725,13 +7754,13 @@
     </row>
     <row r="294" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A294" s="7" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B294" s="9" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C294" s="16" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="D294" s="15"/>
       <c r="E294" s="15"/>
@@ -7742,13 +7771,13 @@
     </row>
     <row r="295" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A295" s="7" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B295" s="9" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C295" s="16" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D295" s="15"/>
       <c r="E295" s="15"/>
@@ -7757,8 +7786,25 @@
         <v>542</v>
       </c>
     </row>
+    <row r="296" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A296" s="7" t="s">
+        <v>556</v>
+      </c>
+      <c r="B296" s="9" t="s">
+        <v>559</v>
+      </c>
+      <c r="C296" s="16" t="s">
+        <v>563</v>
+      </c>
+      <c r="D296" s="15"/>
+      <c r="E296" s="15"/>
+      <c r="F296" s="15"/>
+      <c r="G296" s="1" t="s">
+        <v>542</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A5:G295" xr:uid="{78D23023-8E3A-4FAA-9862-23C6DBAAD3A0}"/>
+  <autoFilter ref="A5:G296" xr:uid="{78D23023-8E3A-4FAA-9862-23C6DBAAD3A0}"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="65" orientation="landscape" r:id="rId1"/>
   <headerFooter>

</xml_diff>